<commit_message>
proses backend belum selesai
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="91">
   <si>
     <t>Rekomendasi proposal</t>
   </si>
@@ -37,6 +37,9 @@
     <t>nomor surat</t>
   </si>
   <si>
+    <t>s_nosurat</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
   </si>
   <si>
     <t>tanggal surat</t>
+  </si>
+  <si>
+    <t>s_tglsurat</t>
   </si>
   <si>
     <t>jenis kelamin</t>
@@ -288,9 +294,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -299,6 +305,82 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -318,110 +400,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -439,12 +422,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -461,13 +467,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,13 +599,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,151 +635,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,23 +679,28 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,13 +744,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,162 +773,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1311,9 +1317,11 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -1323,7 +1331,7 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1331,29 +1339,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1361,19 +1369,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1">
         <v>3</v>
@@ -1383,7 +1391,7 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1391,23 +1399,23 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1415,23 +1423,23 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1">
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1443,11 +1451,11 @@
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1455,21 +1463,23 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G9" s="1">
         <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1481,11 +1491,11 @@
         <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="7:10">
@@ -1493,16 +1503,16 @@
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1511,11 +1521,11 @@
         <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1535,11 +1545,11 @@
         <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1547,11 +1557,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1559,11 +1569,11 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1571,14 +1581,14 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1589,14 +1599,14 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>2</v>
@@ -1616,14 +1626,14 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -1633,7 +1643,7 @@
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1641,11 +1651,11 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G19" s="1">
         <v>2</v>
@@ -1655,7 +1665,7 @@
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1663,24 +1673,24 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G20" s="1">
         <v>3</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1688,24 +1698,24 @@
         <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G21" s="1">
         <v>4</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1713,21 +1723,21 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G22" s="1">
         <v>5</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1735,21 +1745,21 @@
         <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G23" s="1">
         <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1757,21 +1767,21 @@
         <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G24" s="1">
         <v>7</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1779,21 +1789,21 @@
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G25" s="1">
         <v>8</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1801,21 +1811,21 @@
         <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G26" s="1">
         <v>9</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="7:10">
@@ -1823,16 +1833,16 @@
         <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1841,11 +1851,11 @@
         <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1871,7 +1881,7 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1879,14 +1889,14 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1897,11 +1907,11 @@
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>2</v>
@@ -1921,11 +1931,11 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -1935,7 +1945,7 @@
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1943,14 +1953,14 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G34" s="1">
         <v>2</v>
@@ -1960,7 +1970,7 @@
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1968,24 +1978,24 @@
         <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G35" s="1">
         <v>3</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1993,21 +2003,21 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G36" s="1">
         <v>4</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2015,24 +2025,24 @@
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G37" s="1">
         <v>5</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2040,24 +2050,24 @@
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G38" s="1">
         <v>6</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2065,21 +2075,21 @@
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G39" s="1">
         <v>7</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2087,21 +2097,21 @@
         <v>11</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G40" s="1">
         <v>8</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2109,21 +2119,21 @@
         <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G41" s="1">
         <v>9</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2131,21 +2141,21 @@
         <v>13</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G42" s="1">
         <v>10</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2153,21 +2163,21 @@
         <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G43" s="1">
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="7:10">
@@ -2175,16 +2185,16 @@
         <v>12</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2193,11 +2203,11 @@
         <v>13</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2223,7 +2233,7 @@
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2231,14 +2241,14 @@
         <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2249,11 +2259,11 @@
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>2</v>
@@ -2273,11 +2283,11 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G50" s="1">
         <v>1</v>
@@ -2287,7 +2297,7 @@
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2295,11 +2305,11 @@
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G51" s="1">
         <v>2</v>
@@ -2309,7 +2319,7 @@
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2317,24 +2327,24 @@
         <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G52" s="1">
         <v>3</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2342,24 +2352,24 @@
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G53" s="1">
         <v>4</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2367,21 +2377,21 @@
         <v>8</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G54" s="1">
         <v>5</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2389,21 +2399,21 @@
         <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G55" s="1">
         <v>6</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2411,24 +2421,24 @@
         <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G56" s="1">
         <v>7</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2436,24 +2446,24 @@
         <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E57" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G57" s="1">
         <v>8</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2461,21 +2471,21 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G58" s="1">
         <v>9</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2483,21 +2493,21 @@
         <v>13</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G59" s="1">
         <v>10</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2505,21 +2515,21 @@
         <v>14</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G60" s="1">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2527,11 +2537,11 @@
         <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2539,11 +2549,11 @@
         <v>16</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2551,11 +2561,11 @@
         <v>17</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2563,14 +2573,14 @@
         <v>18</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2578,14 +2588,14 @@
         <v>19</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2593,11 +2603,11 @@
         <v>20</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2605,16 +2615,16 @@
         <v>21</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2643,7 +2653,7 @@
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2655,7 +2665,7 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2663,11 +2673,11 @@
         <v>3</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2675,11 +2685,11 @@
         <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2687,11 +2697,11 @@
         <v>5</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2699,14 +2709,14 @@
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2714,14 +2724,14 @@
         <v>7</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2729,11 +2739,11 @@
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2741,11 +2751,11 @@
         <v>9</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2753,11 +2763,11 @@
         <v>10</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2765,11 +2775,11 @@
         <v>11</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2777,11 +2787,11 @@
         <v>12</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2789,11 +2799,11 @@
         <v>13</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2801,11 +2811,11 @@
         <v>14</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2813,11 +2823,11 @@
         <v>15</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2825,11 +2835,11 @@
         <v>16</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2837,11 +2847,11 @@
         <v>17</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2849,11 +2859,11 @@
         <v>18</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2861,16 +2871,16 @@
         <v>19</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2899,7 +2909,7 @@
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2911,7 +2921,7 @@
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2919,11 +2929,11 @@
         <v>3</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2931,14 +2941,14 @@
         <v>4</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E96" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2946,14 +2956,14 @@
         <v>5</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E97" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2961,11 +2971,11 @@
         <v>6</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2973,11 +2983,11 @@
         <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2985,11 +2995,11 @@
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2997,11 +3007,11 @@
         <v>9</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3009,11 +3019,11 @@
         <v>10</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3021,11 +3031,11 @@
         <v>11</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3033,11 +3043,11 @@
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 formulir permohonan ffe
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6975"/>
+    <workbookView windowWidth="8550" windowHeight="7290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="106">
   <si>
     <t>Rekomendasi proposal</t>
   </si>
@@ -58,6 +58,9 @@
     <t>jenis usaha</t>
   </si>
   <si>
+    <t>s_8</t>
+  </si>
+  <si>
     <t>nama pemohon</t>
   </si>
   <si>
@@ -91,6 +94,9 @@
     <t>tanggal lahir</t>
   </si>
   <si>
+    <t>sd_1</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -106,15 +112,24 @@
     <t>pekerjaan</t>
   </si>
   <si>
+    <t>s_5</t>
+  </si>
+  <si>
     <t>alamat jalan</t>
   </si>
   <si>
+    <t>s_6</t>
+  </si>
+  <si>
     <t>Keterangan Domisili</t>
   </si>
   <si>
     <t>alamat rt</t>
   </si>
   <si>
+    <t>s_7</t>
+  </si>
+  <si>
     <t>Nomor surat</t>
   </si>
   <si>
@@ -124,34 +139,19 @@
     <t>11 string</t>
   </si>
   <si>
-    <t>sd_1</t>
-  </si>
-  <si>
     <t>kewarganegaraan</t>
   </si>
   <si>
     <t>agama</t>
   </si>
   <si>
-    <t>s_5</t>
-  </si>
-  <si>
     <t>8 string</t>
   </si>
   <si>
-    <t>s_6</t>
-  </si>
-  <si>
     <t>3 date</t>
   </si>
   <si>
     <t>status perkawinan</t>
-  </si>
-  <si>
-    <t>s_7</t>
-  </si>
-  <si>
-    <t>s_8</t>
   </si>
   <si>
     <t>alamat</t>
@@ -339,10 +339,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -362,6 +362,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -369,7 +385,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,6 +394,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -407,14 +430,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -431,31 +446,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -467,7 +461,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,9 +483,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,7 +512,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,13 +554,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,13 +572,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,13 +584,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,7 +602,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,109 +686,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,6 +717,17 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,15 +780,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -810,11 +812,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,148 +823,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1299,8 +1299,8 @@
   <sheetPr/>
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
@@ -1406,7 +1406,9 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1416,19 +1418,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1">
         <v>3</v>
@@ -1436,7 +1438,9 @@
       <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1446,10 +1450,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -1458,9 +1462,11 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1470,10 +1476,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -1482,9 +1488,11 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1498,11 +1506,13 @@
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1510,21 +1520,23 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G9" s="1">
         <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="J9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1538,9 +1550,11 @@
         <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1550,16 +1564,18 @@
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="J11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1568,9 +1584,11 @@
         <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1592,13 +1610,13 @@
         <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1606,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -1620,10 +1638,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -1634,7 +1652,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>10</v>
@@ -1643,7 +1661,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1654,16 +1672,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>2</v>
@@ -1683,16 +1701,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -1712,10 +1730,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
@@ -1736,22 +1754,22 @@
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G20" s="1">
         <v>3</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
@@ -1763,26 +1781,26 @@
         <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G21" s="1">
         <v>4</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1790,10 +1808,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
@@ -1802,7 +1820,7 @@
         <v>5</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
@@ -1814,10 +1832,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
@@ -1826,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
@@ -1850,7 +1868,7 @@
         <v>7</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
@@ -1886,13 +1904,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G26" s="1">
         <v>9</v>
@@ -1914,7 +1932,7 @@
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1928,13 +1946,13 @@
         <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1968,7 +1986,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
@@ -1986,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
@@ -2010,11 +2028,11 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -2034,14 +2052,14 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G34" s="1">
         <v>2</v>
@@ -2049,7 +2067,9 @@
       <c r="H34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J34" s="1" t="s">
         <v>8</v>
       </c>
@@ -2059,22 +2079,24 @@
         <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G35" s="1">
         <v>3</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="J35" s="1" t="s">
         <v>8</v>
       </c>
@@ -2084,7 +2106,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
@@ -2094,9 +2116,11 @@
         <v>4</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J36" s="1" t="s">
         <v>8</v>
       </c>
@@ -2113,15 +2137,17 @@
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G37" s="1">
         <v>5</v>
       </c>
       <c r="H37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
         <v>8</v>
       </c>
@@ -2138,17 +2164,19 @@
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G38" s="1">
         <v>6</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I38" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J38" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2160,15 +2188,17 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G39" s="1">
         <v>7</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I39" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J39" s="1" t="s">
         <v>8</v>
       </c>
@@ -2188,9 +2218,11 @@
         <v>8</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I40" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="J40" s="1" t="s">
         <v>8</v>
       </c>
@@ -2210,9 +2242,11 @@
         <v>9</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I41" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J41" s="1" t="s">
         <v>8</v>
       </c>
@@ -2232,9 +2266,11 @@
         <v>10</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I42" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J42" s="1" t="s">
         <v>8</v>
       </c>
@@ -2244,11 +2280,11 @@
         <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G43" s="1">
         <v>11</v>
@@ -2256,7 +2292,9 @@
       <c r="H43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="J43" s="1" t="s">
         <v>8</v>
       </c>
@@ -2268,7 +2306,9 @@
       <c r="H44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="J44" s="1" t="s">
         <v>8</v>
       </c>
@@ -2284,13 +2324,13 @@
         <v>13</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2329,7 +2369,7 @@
         <v>63</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>8</v>
@@ -2375,7 +2415,7 @@
         <v>66</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>8</v>
@@ -2401,10 +2441,10 @@
         <v>67</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G51" s="1">
         <v>2</v>
@@ -2413,7 +2453,7 @@
         <v>3</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>8</v>
@@ -2427,7 +2467,7 @@
         <v>68</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
@@ -2439,7 +2479,7 @@
         <v>3</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>10</v>
@@ -2456,22 +2496,22 @@
         <v>69</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G53" s="1">
         <v>4</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>8</v>
@@ -2485,7 +2525,7 @@
         <v>70</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>8</v>
@@ -2494,10 +2534,10 @@
         <v>5</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>8</v>
@@ -2511,7 +2551,7 @@
         <v>71</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
@@ -2520,13 +2560,13 @@
         <v>6</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2537,7 +2577,7 @@
         <v>72</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
@@ -2549,10 +2589,10 @@
         <v>7</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>8</v>
@@ -2569,7 +2609,7 @@
         <v>75</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E57" t="s">
         <v>76</v>
@@ -2578,10 +2618,10 @@
         <v>8</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>8</v>
@@ -2607,7 +2647,7 @@
         <v>46</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>8</v>
@@ -2633,7 +2673,7 @@
         <v>79</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>8</v>
@@ -2656,13 +2696,13 @@
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2704,7 +2744,7 @@
         <v>87</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2760,13 +2800,13 @@
         <v>21</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2820,7 +2860,7 @@
         <v>3</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
@@ -2832,7 +2872,7 @@
         <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
@@ -2844,11 +2884,11 @@
         <v>5</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2856,7 +2896,7 @@
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
@@ -2871,14 +2911,14 @@
         <v>7</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2886,7 +2926,7 @@
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
@@ -2898,7 +2938,7 @@
         <v>9</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
@@ -2934,7 +2974,7 @@
         <v>12</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
@@ -3010,7 +3050,7 @@
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3018,11 +3058,11 @@
         <v>19</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3054,7 +3094,9 @@
       <c r="B93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C93" s="1"/>
+      <c r="C93" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D93" s="1" t="s">
         <v>8</v>
       </c>
@@ -3066,7 +3108,9 @@
       <c r="B94" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C94" s="1"/>
+      <c r="C94" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D94" s="1" t="s">
         <v>8</v>
       </c>
@@ -3076,9 +3120,11 @@
         <v>3</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D95" s="1" t="s">
         <v>8</v>
       </c>
@@ -3088,9 +3134,11 @@
         <v>4</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
         <v>8</v>
       </c>
@@ -3103,14 +3151,16 @@
         <v>5</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C97" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D97" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E97" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3118,9 +3168,11 @@
         <v>6</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C98" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D98" s="1" t="s">
         <v>8</v>
       </c>
@@ -3130,9 +3182,11 @@
         <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C99" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D99" s="1" t="s">
         <v>8</v>
       </c>
@@ -3142,9 +3196,11 @@
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C100" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D100" s="1" t="s">
         <v>8</v>
       </c>
@@ -3154,9 +3210,11 @@
         <v>9</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C101" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D101" s="1" t="s">
         <v>8</v>
       </c>
@@ -3166,9 +3224,11 @@
         <v>10</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C102" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D102" s="1" t="s">
         <v>8</v>
       </c>
@@ -3180,7 +3240,9 @@
       <c r="B103" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C103" s="1"/>
+      <c r="C103" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D103" s="1" t="s">
         <v>8</v>
       </c>
@@ -3190,11 +3252,13 @@
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C104" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D104" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fe selesai kurang nikah
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8550" windowHeight="7290"/>
+    <workbookView windowWidth="19200" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="106">
   <si>
     <t>Rekomendasi proposal</t>
   </si>
@@ -175,6 +175,9 @@
     <t>tanggal hilang</t>
   </si>
   <si>
+    <t>sd_2</t>
+  </si>
+  <si>
     <t>Keterangan Kematian</t>
   </si>
   <si>
@@ -239,9 +242,6 @@
   </si>
   <si>
     <t>tanggal lahir ayah</t>
-  </si>
-  <si>
-    <t>sd_2</t>
   </si>
   <si>
     <t>4 date</t>
@@ -339,10 +339,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -353,16 +353,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -376,16 +375,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,8 +413,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,7 +469,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,14 +484,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -484,14 +491,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,7 +512,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,7 +560,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,7 +644,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,145 +686,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,6 +717,45 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -756,26 +795,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,36 +818,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -832,139 +838,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1299,8 +1299,8 @@
   <sheetPr/>
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
@@ -1744,7 +1744,9 @@
       <c r="H19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1771,7 +1773,9 @@
       <c r="H20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1798,7 +1802,9 @@
       <c r="H21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1822,7 +1828,9 @@
       <c r="H22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="J22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1846,7 +1854,9 @@
       <c r="H23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="J23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1870,7 +1880,9 @@
       <c r="H24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1894,7 +1906,9 @@
       <c r="H25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="J25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1918,7 +1932,9 @@
       <c r="H26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1930,14 +1946,16 @@
       <c r="H27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="J27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1993,7 +2011,7 @@
         <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2130,7 +2148,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
@@ -2157,7 +2175,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
@@ -2184,7 +2202,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
@@ -2208,7 +2226,7 @@
         <v>11</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
@@ -2232,7 +2250,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
@@ -2256,7 +2274,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
@@ -2304,7 +2322,7 @@
         <v>12</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>49</v>
@@ -2315,7 +2333,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2366,7 +2384,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>16</v>
@@ -2375,7 +2393,7 @@
         <v>8</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2386,7 +2404,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>10</v>
@@ -2412,7 +2430,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>20</v>
@@ -2438,7 +2456,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>26</v>
@@ -2464,7 +2482,7 @@
         <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>23</v>
@@ -2493,7 +2511,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>32</v>
@@ -2522,7 +2540,7 @@
         <v>8</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>34</v>
@@ -2548,7 +2566,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>37</v>
@@ -2574,7 +2592,7 @@
         <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>14</v>
@@ -2583,7 +2601,7 @@
         <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G56" s="1">
         <v>7</v>
@@ -2603,10 +2621,10 @@
         <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>27</v>
@@ -2761,7 +2779,7 @@
         <v>8</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2838,7 +2856,9 @@
       <c r="B71" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="1"/>
+      <c r="C71" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
       </c>
@@ -2850,7 +2870,9 @@
       <c r="B72" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C72" s="1"/>
+      <c r="C72" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
       </c>
@@ -2862,7 +2884,9 @@
       <c r="B73" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C73" s="1"/>
+      <c r="C73" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
       </c>
@@ -2874,7 +2898,9 @@
       <c r="B74" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C74" s="1"/>
+      <c r="C74" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
       </c>
@@ -2886,7 +2912,9 @@
       <c r="B75" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C75" s="1"/>
+      <c r="C75" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D75" s="1" t="s">
         <v>27</v>
       </c>
@@ -2898,7 +2926,9 @@
       <c r="B76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C76" s="1"/>
+      <c r="C76" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D76" s="1" t="s">
         <v>8</v>
       </c>
@@ -2913,7 +2943,9 @@
       <c r="B77" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D77" s="1" t="s">
         <v>8</v>
       </c>
@@ -2928,7 +2960,9 @@
       <c r="B78" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C78" s="1"/>
+      <c r="C78" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D78" s="1" t="s">
         <v>8</v>
       </c>
@@ -2940,7 +2974,9 @@
       <c r="B79" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C79" s="1"/>
+      <c r="C79" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D79" s="1" t="s">
         <v>8</v>
       </c>
@@ -2952,7 +2988,9 @@
       <c r="B80" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C80" s="1"/>
+      <c r="C80" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D80" s="1" t="s">
         <v>8</v>
       </c>
@@ -2964,7 +3002,9 @@
       <c r="B81" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="1"/>
+      <c r="C81" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D81" s="1" t="s">
         <v>8</v>
       </c>
@@ -2976,7 +3016,9 @@
       <c r="B82" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C82" s="1"/>
+      <c r="C82" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D82" s="1" t="s">
         <v>8</v>
       </c>
@@ -2988,7 +3030,9 @@
       <c r="B83" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C83" s="1"/>
+      <c r="C83" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D83" s="1" t="s">
         <v>8</v>
       </c>
@@ -3000,7 +3044,9 @@
       <c r="B84" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C84" s="1"/>
+      <c r="C84" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D84" s="1" t="s">
         <v>8</v>
       </c>
@@ -3012,7 +3058,9 @@
       <c r="B85" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C85" s="1"/>
+      <c r="C85" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="D85" s="1" t="s">
         <v>8</v>
       </c>
@@ -3024,7 +3072,9 @@
       <c r="B86" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C86" s="1"/>
+      <c r="C86" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="D86" s="1" t="s">
         <v>8</v>
       </c>
@@ -3036,7 +3086,9 @@
       <c r="B87" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C87" s="1"/>
+      <c r="C87" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D87" s="1" t="s">
         <v>8</v>
       </c>
@@ -3048,7 +3100,9 @@
       <c r="B88" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C88" s="1"/>
+      <c r="C88" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D88" s="1" t="s">
         <v>27</v>
       </c>
@@ -3060,7 +3114,9 @@
       <c r="B89" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C89" s="1"/>
+      <c r="C89" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D89" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
buat surat manual be
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8550" windowHeight="6825"/>
+    <workbookView windowWidth="19200" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="106">
   <si>
     <t>Rekomendasi proposal</t>
   </si>
@@ -339,10 +339,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -367,24 +367,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,24 +390,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,14 +428,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -468,10 +444,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -484,14 +469,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,43 +512,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,43 +542,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,7 +560,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,19 +668,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,49 +686,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -721,30 +721,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -762,11 +738,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,9 +771,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -818,161 +803,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1302,8 +1299,8 @@
   <sheetPr/>
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
@@ -1635,16 +1632,16 @@
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>12</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2301,9 +2298,7 @@
       <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
@@ -2822,7 +2817,7 @@
       <c r="D64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2839,7 +2834,7 @@
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="2" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>